<commit_message>
choosingplayers is almost done. But selections have locked up for the day, so have to suspend work
</commit_message>
<xml_diff>
--- a/btsAccountsTest.xlsx
+++ b/btsAccountsTest.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="20" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620"/>
   </bookViews>
   <sheets>
     <sheet name="Production" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,37 +21,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>EmailPassword</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>EmailPassword</t>
-  </si>
-  <si>
     <t>MLBPassword</t>
   </si>
   <si>
+    <t>beatthestreak1</t>
+  </si>
+  <si>
     <t>faiyam@faiyamrahman.com</t>
   </si>
   <si>
+    <t>fossil.williams.1140@faiyamrahman.com</t>
+  </si>
+  <si>
     <t>n/a</t>
-  </si>
-  <si>
-    <t>beatthestreak1</t>
-  </si>
-  <si>
-    <t>fossil.williams.1140@faiyamrahman.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -63,6 +63,22 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,8 +113,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -106,11 +124,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -189,7 +209,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -224,7 +243,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -259,16 +277,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -390,46 +412,7 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
@@ -439,26 +422,20 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -469,13 +446,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -483,17 +460,18 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
chooseplayers.py is now fully operational on a two player test case running on MAC OSX MAvericks
</commit_message>
<xml_diff>
--- a/btsAccountsTest.xlsx
+++ b/btsAccountsTest.xlsx
@@ -19,7 +19,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>7-8</t>
+  </si>
+  <si>
+    <t>Done. 1: ('Giancarlo', 'Stanton', 'Miami Marlins'), 2: ('Adam', 'Lind', 'Toronto Blue Jays')</t>
+  </si>
+  <si>
+    <t>Done. 1: ('Yasiel', 'Puig', 'Los Angeles Dodgers'), 2: ('Adam', 'Lind', 'Toronto Blue Jays')</t>
+  </si>
   <si>
     <t>Email</t>
   </si>
@@ -49,7 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,22 +72,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,10 +106,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -124,9 +115,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,59 +408,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
+      <c r="E2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
+      <c r="E3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
just run chooseplayers on google linux box with btsAccountsTest10. Committing to view excel file and see if everything worked
</commit_message>
<xml_diff>
--- a/btsAccountsTest.xlsx
+++ b/btsAccountsTest.xlsx
@@ -1,33 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Production" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Production" sheetId="1" r:id="rId1"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>7-8</t>
   </si>
   <si>
-    <t>Done. 1: ('Giancarlo', 'Stanton', 'Miami Marlins'), 2: ('Adam', 'Lind', 'Toronto Blue Jays')</t>
-  </si>
-  <si>
-    <t>Done. 1: ('Yasiel', 'Puig', 'Los Angeles Dodgers'), 2: ('Adam', 'Lind', 'Toronto Blue Jays')</t>
+    <t>Done. 1: ('Adam', 'Lind', 'Toronto Blue Jays'), 2: ('Yasiel', 'Puig', 'Los Angeles Dodgers')</t>
+  </si>
+  <si>
+    <t>Done. 1: ('Robinson', 'Cano', 'Seattle Mariners'), 2: ('Adam', 'Lind', 'Toronto Blue Jays')</t>
   </si>
   <si>
     <t>Email</t>
@@ -57,8 +53,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,11 +64,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,19 +104,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -128,10 +125,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -287,7 +284,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -296,13 +293,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -312,7 +309,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -321,7 +318,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -330,7 +327,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -340,12 +337,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -376,7 +373,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -395,7 +392,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -407,79 +404,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.83203125" bestFit="1" customWidth="1"/>
+    <col width="9.10" min="1" max="1"/>
+    <col width="9.10" min="2" max="2"/>
+    <col width="9.10" min="3" max="3"/>
+    <col width="9.10" min="4" max="4"/>
+    <col width="9.10" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row spans="1:5" r="1">
+      <c t="s" s="1" r="A1">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c t="s" s="1" r="B1">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c t="s" s="1" r="C1">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c t="s" s="1" r="D1">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c t="s" s="1" r="E1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
+    <row spans="1:5" r="2">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c t="s" r="D2">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row spans="1:5" r="3">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="s" r="B3">
+        <v>9</v>
+      </c>
+      <c t="s" r="C3">
+        <v>10</v>
+      </c>
+      <c t="s" r="D3">
+        <v>7</v>
+      </c>
+      <c t="s" r="E3">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chooseplayers is now modularized with respect to selection and distribution of players
</commit_message>
<xml_diff>
--- a/btsAccountsTest.xlsx
+++ b/btsAccountsTest.xlsx
@@ -15,17 +15,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>7-8</t>
   </si>
   <si>
+    <t>7-9</t>
+  </si>
+  <si>
     <t>Done. 1: ('Adam', 'Lind', 'Toronto Blue Jays'), 2: ('Yasiel', 'Puig', 'Los Angeles Dodgers')</t>
   </si>
   <si>
     <t>Done. 1: ('Robinson', 'Cano', 'Seattle Mariners'), 2: ('Adam', 'Lind', 'Toronto Blue Jays')</t>
   </si>
   <si>
+    <t>Done. 1: ('Robinson', 'Cano', 'sea'), 2: ()</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
@@ -36,6 +42,15 @@
   </si>
   <si>
     <t>MLBPassword</t>
+  </si>
+  <si>
+    <t>NOT DONE</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>VM</t>
   </si>
   <si>
     <t>beatthestreak1</t>
@@ -404,11 +419,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -416,62 +431,92 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.10" min="1" max="1"/>
-    <col width="9.10" min="2" max="2"/>
-    <col width="9.10" min="3" max="3"/>
-    <col width="9.10" min="4" max="4"/>
-    <col width="9.10" min="5" max="5"/>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
+    <col min="3" max="3" width="9.10"/>
+    <col min="4" max="4" width="9.10"/>
+    <col min="5" max="5" width="9.10"/>
+    <col min="6" max="6" width="9.10"/>
+    <col min="7" max="7" width="9.10"/>
+    <col min="8" max="8" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:5" r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:8">
+      <c s="1" r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c s="1" r="B1" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c s="1" r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c s="1" r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c s="1" r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c s="1" r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c s="1" r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c s="1" r="H1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="1" r="C1">
-        <v>4</v>
-      </c>
-      <c t="s" s="1" r="D1">
-        <v>6</v>
-      </c>
-      <c t="s" s="1" r="E1">
-        <v>0</v>
-      </c>
-    </row>
-    <row spans="1:5" r="2">
-      <c t="n" r="A2">
-        <v>0</v>
-      </c>
-      <c t="s" r="B2">
-        <v>8</v>
-      </c>
-      <c t="s" r="C2">
-        <v>10</v>
-      </c>
-      <c t="s" r="D2">
-        <v>7</v>
-      </c>
-      <c t="s" r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:5" r="3">
-      <c t="n" r="A3">
-        <v>1</v>
-      </c>
-      <c t="s" r="B3">
+      <c r="H3" t="s">
         <v>9</v>
-      </c>
-      <c t="s" r="C3">
-        <v>10</v>
-      </c>
-      <c t="s" r="D3">
-        <v>7</v>
-      </c>
-      <c t="s" r="E3">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modularized choose_players even more so now it has a seperate reporting function. Very close to being production ready for 1000 accounts on strategy 5. Still need to tweak reporting from individual VMs and gathering all the data later, and need to figure out how to operate everything from a central terminal and not fall prey to broken pipes-.-
</commit_message>
<xml_diff>
--- a/btsAccountsTest.xlsx
+++ b/btsAccountsTest.xlsx
@@ -29,7 +29,10 @@
     <t>Done. 1: ('Robinson', 'Cano', 'Seattle Mariners'), 2: ('Adam', 'Lind', 'Toronto Blue Jays')</t>
   </si>
   <si>
-    <t>Done. 1: ('Robinson', 'Cano', 'sea'), 2: ()</t>
+    <t>Done. 1: ('Robinson', 'Cano', 'sea'), 2: ('Michael', 'Brantley', 'cle')</t>
+  </si>
+  <si>
+    <t>Done. 1: ('Troy', 'Tulowitzki', 'col'), 2: ()</t>
   </si>
   <si>
     <t>Email</t>
@@ -42,9 +45,6 @@
   </si>
   <si>
     <t>MLBPassword</t>
-  </si>
-  <si>
-    <t>NOT DONE</t>
   </si>
   <si>
     <t>Strategy</t>
@@ -443,16 +443,16 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c s="1" r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c s="1" r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c s="1" r="C1" t="s">
         <v>7</v>
       </c>
-      <c s="1" r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c s="1" r="C1" t="s">
-        <v>6</v>
-      </c>
       <c s="1" r="D1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c s="1" r="E1" t="s">
         <v>10</v>
@@ -516,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debugged the problem with danging displays in accounts.py
</commit_message>
<xml_diff>
--- a/btsAccountsTest.xlsx
+++ b/btsAccountsTest.xlsx
@@ -15,25 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
-  <si>
-    <t>7-8</t>
-  </si>
-  <si>
-    <t>7-9</t>
-  </si>
-  <si>
-    <t>Done. 1: ('Adam', 'Lind', 'Toronto Blue Jays'), 2: ('Yasiel', 'Puig', 'Los Angeles Dodgers')</t>
-  </si>
-  <si>
-    <t>Done. 1: ('Robinson', 'Cano', 'Seattle Mariners'), 2: ('Adam', 'Lind', 'Toronto Blue Jays')</t>
-  </si>
-  <si>
-    <t>Done. 1: ('Robinson', 'Cano', 'sea'), 2: ('Michael', 'Brantley', 'cle')</t>
-  </si>
-  <si>
-    <t>Done. 1: ('Troy', 'Tulowitzki', 'col'), 2: ()</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>Email</t>
   </si>
@@ -47,15 +29,12 @@
     <t>MLBPassword</t>
   </si>
   <si>
-    <t>Strategy</t>
-  </si>
-  <si>
-    <t>VM</t>
-  </si>
-  <si>
     <t>beatthestreak1</t>
   </si>
   <si>
+    <t>faiyam.daft.154@faiyamrahman.com</t>
+  </si>
+  <si>
     <t>faiyam@faiyamrahman.com</t>
   </si>
   <si>
@@ -63,6 +42,9 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>water.water.354@faiyamrahman.com</t>
   </si>
 </sst>
 </file>
@@ -419,11 +401,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -431,92 +413,80 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
-    <col min="3" max="3" width="9.10"/>
-    <col min="4" max="4" width="9.10"/>
-    <col min="5" max="5" width="9.10"/>
-    <col min="6" max="6" width="9.10"/>
-    <col min="7" max="7" width="9.10"/>
-    <col min="8" max="8" width="9.10"/>
+    <col width="9.10" min="1" max="1"/>
+    <col width="9.10" min="2" max="2"/>
+    <col width="9.10" min="3" max="3"/>
+    <col width="9.10" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c s="1" r="A1" t="s">
+    <row spans="1:4" r="1">
+      <c t="s" s="1" r="A1">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>0</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>1</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>3</v>
+      </c>
+    </row>
+    <row spans="1:4" r="2">
+      <c t="n" r="A2">
+        <v>0</v>
+      </c>
+      <c t="s" r="B2">
+        <v>6</v>
+      </c>
+      <c t="s" r="C2">
         <v>8</v>
       </c>
-      <c s="1" r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c s="1" r="C1" t="s">
+      <c t="s" r="D2">
+        <v>4</v>
+      </c>
+    </row>
+    <row spans="1:4" r="3">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="s" r="B3">
         <v>7</v>
       </c>
-      <c s="1" r="D1" t="s">
+      <c t="s" r="C3">
+        <v>8</v>
+      </c>
+      <c t="s" r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row spans="1:4" r="4">
+      <c t="n" r="A4">
+        <v>2</v>
+      </c>
+      <c t="s" r="B4">
+        <v>5</v>
+      </c>
+      <c t="s" r="C4">
+        <v>8</v>
+      </c>
+      <c t="s" r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row spans="1:4" r="5">
+      <c t="n" r="A5">
+        <v>3</v>
+      </c>
+      <c t="s" r="B5">
         <v>9</v>
       </c>
-      <c s="1" r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c s="1" r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c s="1" r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c s="1" r="H1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
+      <c t="s" r="C5">
+        <v>8</v>
+      </c>
+      <c t="s" r="D5">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>